<commit_message>
All besides "other covariates" done
</commit_message>
<xml_diff>
--- a/Output/AllModels_sensPlan.xlsx
+++ b/Output/AllModels_sensPlan.xlsx
@@ -1,1289 +1,1282 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kueng\DataAnalysis\02TimeAndTiesControl_updatedBRMS\Output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E493B97C-8F15-4F2C-B8E4-F15746F4FCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-19303" yWindow="3369" windowWidth="19406" windowHeight="11485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="419">
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Subjective MVPA Hurdle Lognormal</t>
-  </si>
-  <si>
-    <t>Device-Based MVPA Log (Gaussian)</t>
-  </si>
-  <si>
-    <t>Mood Gaussian</t>
-  </si>
-  <si>
-    <t>Reactance Ordinal</t>
-  </si>
-  <si>
-    <t>Reactance Dichotome</t>
-  </si>
-  <si>
-    <t>exp(Est.)</t>
-  </si>
-  <si>
-    <t>95% CI</t>
-  </si>
-  <si>
-    <t>pd</t>
-  </si>
-  <si>
-    <t>Est.</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>Intercept</t>
-  </si>
-  <si>
-    <t>38.50***</t>
-  </si>
-  <si>
-    <t>[33.71, 44.19]</t>
-  </si>
-  <si>
-    <t>1.000</t>
-  </si>
-  <si>
-    <t>112.69***</t>
-  </si>
-  <si>
-    <t>[101.42, 125.34]</t>
-  </si>
-  <si>
-    <t>3.66***</t>
-  </si>
-  <si>
-    <t>[ 3.44, 3.88]</t>
-  </si>
-  <si>
-    <t>0.32***</t>
-  </si>
-  <si>
-    <t>[0.16,   0.61]</t>
-  </si>
-  <si>
-    <t>Hurdle Intercept</t>
-  </si>
-  <si>
-    <t>0.27***</t>
-  </si>
-  <si>
-    <t>[ 0.20,  0.37]</t>
-  </si>
-  <si>
-    <t>Conditional Within-Person Effects</t>
-  </si>
-  <si>
-    <t>Daily persuasion experienced</t>
-  </si>
-  <si>
-    <t>1.03</t>
-  </si>
-  <si>
-    <t>[ 0.98,  1.09]</t>
-  </si>
-  <si>
-    <t>0.879</t>
-  </si>
-  <si>
-    <t>[  1.00,   1.06]</t>
-  </si>
-  <si>
-    <t>0.957</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>[-0.04, 0.05]</t>
-  </si>
-  <si>
-    <t>0.526</t>
-  </si>
-  <si>
-    <t>0.85*</t>
-  </si>
-  <si>
-    <t>[   0.72,     1.00]</t>
-  </si>
-  <si>
-    <t>0.977</t>
-  </si>
-  <si>
-    <t>0.85</t>
-  </si>
-  <si>
-    <t>[0.70,   1.01]</t>
-  </si>
-  <si>
-    <t>0.968</t>
-  </si>
-  <si>
-    <t>Daily persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>[ 0.99,  1.08]</t>
-  </si>
-  <si>
-    <t>0.921</t>
-  </si>
-  <si>
-    <t>1.02</t>
-  </si>
-  <si>
-    <t>[  0.99,   1.05]</t>
-  </si>
-  <si>
-    <t>0.869</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>[-0.02, 0.07]</t>
-  </si>
-  <si>
-    <t>0.827</t>
-  </si>
-  <si>
-    <t>[   0.83,     1.24]</t>
-  </si>
-  <si>
-    <t>0.589</t>
-  </si>
-  <si>
-    <t>1.11</t>
-  </si>
-  <si>
-    <t>[0.82,   1.52]</t>
-  </si>
-  <si>
-    <t>0.760</t>
-  </si>
-  <si>
-    <t>Daily pressure experienced</t>
-  </si>
-  <si>
-    <t>0.91</t>
-  </si>
-  <si>
-    <t>[ 0.82,  1.00]</t>
-  </si>
-  <si>
-    <t>0.971</t>
-  </si>
-  <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>[  0.89,   1.01]</t>
-  </si>
-  <si>
-    <t>0.938</t>
-  </si>
-  <si>
-    <t>-0.03</t>
-  </si>
-  <si>
-    <t>[-0.14, 0.07]</t>
-  </si>
-  <si>
-    <t>0.703</t>
-  </si>
-  <si>
-    <t>1.83*</t>
-  </si>
-  <si>
-    <t>[   1.14,     2.59]</t>
-  </si>
-  <si>
-    <t>0.994</t>
-  </si>
-  <si>
-    <t>1.96*</t>
-  </si>
-  <si>
-    <t>[1.00,   4.44]</t>
-  </si>
-  <si>
-    <t>0.976</t>
-  </si>
-  <si>
-    <t>Daily pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>0.94</t>
-  </si>
-  <si>
-    <t>[ 0.86,  1.02]</t>
-  </si>
-  <si>
-    <t>0.923</t>
-  </si>
-  <si>
-    <t>0.98</t>
-  </si>
-  <si>
-    <t>[  0.92,   1.05]</t>
-  </si>
-  <si>
-    <t>0.735</t>
-  </si>
-  <si>
-    <t>[-0.15, 0.08]</t>
-  </si>
-  <si>
-    <t>0.699</t>
-  </si>
-  <si>
-    <t>1.24</t>
-  </si>
-  <si>
-    <t>[   0.70,     2.13]</t>
-  </si>
-  <si>
-    <t>0.810</t>
-  </si>
-  <si>
-    <t>1.44</t>
-  </si>
-  <si>
-    <t>[0.60,   4.93]</t>
-  </si>
-  <si>
-    <t>0.819</t>
-  </si>
-  <si>
-    <t>Daily pushing experienced</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>[ 0.92,  1.05]</t>
-  </si>
-  <si>
-    <t>0.672</t>
-  </si>
-  <si>
-    <t>[  0.97,   1.07]</t>
-  </si>
-  <si>
-    <t>0.738</t>
-  </si>
-  <si>
-    <t>[-0.06, 0.07]</t>
-  </si>
-  <si>
-    <t>0.550</t>
-  </si>
-  <si>
-    <t>1.21</t>
-  </si>
-  <si>
-    <t>[   0.97,     1.52]</t>
-  </si>
-  <si>
-    <t>0.962</t>
-  </si>
-  <si>
-    <t>1.33*</t>
-  </si>
-  <si>
-    <t>[1.02,   1.76]</t>
-  </si>
-  <si>
-    <t>0.980</t>
-  </si>
-  <si>
-    <t>Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>[ 0.91,  1.03]</t>
-  </si>
-  <si>
-    <t>0.832</t>
-  </si>
-  <si>
-    <t>1.01</t>
-  </si>
-  <si>
-    <t>[  0.96,   1.05]</t>
-  </si>
-  <si>
-    <t>0.608</t>
-  </si>
-  <si>
-    <t>0.07</t>
-  </si>
-  <si>
-    <t>[ 0.00, 0.13]</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>[   0.72,     1.20]</t>
-  </si>
-  <si>
-    <t>0.739</t>
-  </si>
-  <si>
-    <t>[0.61,   1.35]</t>
-  </si>
-  <si>
-    <t>0.694</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>[ 0.88,  1.12]</t>
-  </si>
-  <si>
-    <t>[  0.91,   1.04]</t>
-  </si>
-  <si>
-    <t>0.796</t>
-  </si>
-  <si>
-    <t>0.26***</t>
-  </si>
-  <si>
-    <t>[ 0.15, 0.37]</t>
-  </si>
-  <si>
-    <t>1.48</t>
-  </si>
-  <si>
-    <t>[   0.75,     2.89]</t>
-  </si>
-  <si>
-    <t>0.864</t>
-  </si>
-  <si>
-    <t>1.64</t>
-  </si>
-  <si>
-    <t>[0.74,   3.49]</t>
-  </si>
-  <si>
-    <t>0.892</t>
-  </si>
-  <si>
-    <t>Daily weartime</t>
-  </si>
-  <si>
-    <t>1.00***</t>
-  </si>
-  <si>
-    <t>[  1.00,   1.00]</t>
-  </si>
-  <si>
-    <t>Actionplan</t>
-  </si>
-  <si>
-    <t>1.37***</t>
-  </si>
-  <si>
-    <t>[ 1.25,  1.49]</t>
-  </si>
-  <si>
-    <t>1.09**</t>
-  </si>
-  <si>
-    <t>[  1.04,   1.14]</t>
-  </si>
-  <si>
-    <t>0.09**</t>
-  </si>
-  <si>
-    <t>[ 0.02, 0.16]</t>
-  </si>
-  <si>
-    <t>0.997</t>
-  </si>
-  <si>
-    <t>0.84</t>
-  </si>
-  <si>
-    <t>[   0.51,     1.37]</t>
-  </si>
-  <si>
-    <t>0.752</t>
-  </si>
-  <si>
-    <t>0.83</t>
-  </si>
-  <si>
-    <t>[0.49,   1.43]</t>
-  </si>
-  <si>
-    <t>0.756</t>
-  </si>
-  <si>
-    <t>Daily support received</t>
-  </si>
-  <si>
-    <t>Daily support provided (partner's view)</t>
-  </si>
-  <si>
-    <t>Is a Weekend</t>
-  </si>
-  <si>
-    <t>JITAI received</t>
-  </si>
-  <si>
-    <t>Days post skilled support intervention</t>
-  </si>
-  <si>
-    <t>Conditional Between-Person Effects</t>
-  </si>
-  <si>
-    <t>Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t>[ 0.70,  1.29]</t>
-  </si>
-  <si>
-    <t>0.660</t>
-  </si>
-  <si>
-    <t>1.06</t>
-  </si>
-  <si>
-    <t>[  0.79,   1.41]</t>
-  </si>
-  <si>
-    <t>0.658</t>
-  </si>
-  <si>
-    <t>0.24</t>
-  </si>
-  <si>
-    <t>[-0.35, 0.80]</t>
-  </si>
-  <si>
-    <t>0.799</t>
-  </si>
-  <si>
-    <t>1.27</t>
-  </si>
-  <si>
-    <t>[   0.44,     3.81]</t>
-  </si>
-  <si>
-    <t>0.678</t>
-  </si>
-  <si>
-    <t>2.04</t>
-  </si>
-  <si>
-    <t>[0.63,   7.27]</t>
-  </si>
-  <si>
-    <t>0.878</t>
-  </si>
-  <si>
-    <t>Mean persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>[ 0.75,  1.36]</t>
-  </si>
-  <si>
-    <t>0.509</t>
-  </si>
-  <si>
-    <t>[  0.73,   1.31]</t>
-  </si>
-  <si>
-    <t>0.570</t>
-  </si>
-  <si>
-    <t>0.31</t>
-  </si>
-  <si>
-    <t>[-0.27, 0.87]</t>
-  </si>
-  <si>
-    <t>0.857</t>
-  </si>
-  <si>
-    <t>1.43</t>
-  </si>
-  <si>
-    <t>[   0.46,     5.12]</t>
-  </si>
-  <si>
-    <t>0.737</t>
-  </si>
-  <si>
-    <t>2.01</t>
-  </si>
-  <si>
-    <t>[0.53,   7.95]</t>
-  </si>
-  <si>
-    <t>0.841</t>
-  </si>
-  <si>
-    <t>Mean pressure experienced</t>
-  </si>
-  <si>
-    <t>1.23</t>
-  </si>
-  <si>
-    <t>[ 0.87,  1.72]</t>
-  </si>
-  <si>
-    <t>0.875</t>
-  </si>
-  <si>
-    <t>[  0.77,   1.37]</t>
-  </si>
-  <si>
-    <t>0.544</t>
-  </si>
-  <si>
-    <t>-0.25</t>
-  </si>
-  <si>
-    <t>[-0.81, 0.32]</t>
-  </si>
-  <si>
-    <t>0.808</t>
-  </si>
-  <si>
-    <t>3.49*</t>
-  </si>
-  <si>
-    <t>[   1.13,    10.80]</t>
-  </si>
-  <si>
-    <t>0.986</t>
-  </si>
-  <si>
-    <t>19.45**</t>
-  </si>
-  <si>
-    <t>[2.52, 170.41]</t>
-  </si>
-  <si>
-    <t>0.998</t>
-  </si>
-  <si>
-    <t>Mean pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>[ 0.65,  1.33]</t>
-  </si>
-  <si>
-    <t>0.643</t>
-  </si>
-  <si>
-    <t>0.96</t>
-  </si>
-  <si>
-    <t>[  0.73,   1.28]</t>
-  </si>
-  <si>
-    <t>0.597</t>
-  </si>
-  <si>
-    <t>-0.35</t>
-  </si>
-  <si>
-    <t>[-0.89, 0.20]</t>
-  </si>
-  <si>
-    <t>0.891</t>
-  </si>
-  <si>
-    <t>1.13</t>
-  </si>
-  <si>
-    <t>[   0.35,     3.45]</t>
-  </si>
-  <si>
-    <t>0.583</t>
-  </si>
-  <si>
-    <t>2.47</t>
-  </si>
-  <si>
-    <t>[0.23,  22.98]</t>
-  </si>
-  <si>
-    <t>0.785</t>
-  </si>
-  <si>
-    <t>Mean pushing experienced</t>
-  </si>
-  <si>
-    <t>1.19</t>
-  </si>
-  <si>
-    <t>[ 0.72,  1.90]</t>
-  </si>
-  <si>
-    <t>0.769</t>
-  </si>
-  <si>
-    <t>[  0.59,   1.48]</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>[-0.57, 1.03]</t>
-  </si>
-  <si>
-    <t>0.732</t>
-  </si>
-  <si>
-    <t>1.79</t>
-  </si>
-  <si>
-    <t>[   0.36,     9.61]</t>
-  </si>
-  <si>
-    <t>0.754</t>
-  </si>
-  <si>
-    <t>1.25</t>
-  </si>
-  <si>
-    <t>[0.16,   9.49]</t>
-  </si>
-  <si>
-    <t>0.591</t>
-  </si>
-  <si>
-    <t>Mean pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>1.07</t>
-  </si>
-  <si>
-    <t>[ 0.65,  1.74]</t>
-  </si>
-  <si>
-    <t>0.622</t>
-  </si>
-  <si>
-    <t>[  0.73,   1.83]</t>
-  </si>
-  <si>
-    <t>0.673</t>
-  </si>
-  <si>
-    <t>0.21</t>
-  </si>
-  <si>
-    <t>[-0.62, 1.01]</t>
-  </si>
-  <si>
-    <t>0.693</t>
-  </si>
-  <si>
-    <t>0.15</t>
-  </si>
-  <si>
-    <t>[   0.02,     1.00]</t>
-  </si>
-  <si>
-    <t>0.975</t>
-  </si>
-  <si>
-    <t>0.10*</t>
-  </si>
-  <si>
-    <t>[0.01,   0.84]</t>
-  </si>
-  <si>
-    <t>0.982</t>
-  </si>
-  <si>
-    <t>Mean weartime</t>
-  </si>
-  <si>
-    <t>0.944</t>
-  </si>
-  <si>
-    <t>Mean support received</t>
-  </si>
-  <si>
-    <t>1.14**</t>
-  </si>
-  <si>
-    <t>[ 1.04,  1.25]</t>
-  </si>
-  <si>
-    <t>[  0.98,   1.16]</t>
-  </si>
-  <si>
-    <t>0.942</t>
-  </si>
-  <si>
-    <t>0.14</t>
-  </si>
-  <si>
-    <t>[-0.01, 0.30]</t>
-  </si>
-  <si>
-    <t>0.961</t>
-  </si>
-  <si>
-    <t>0.73</t>
-  </si>
-  <si>
-    <t>[   0.41,     1.31]</t>
-  </si>
-  <si>
-    <t>0.859</t>
-  </si>
-  <si>
-    <t>0.77</t>
-  </si>
-  <si>
-    <t>[0.39,   1.46]</t>
-  </si>
-  <si>
-    <t>0.775</t>
-  </si>
-  <si>
-    <t>Mean support provided (partner's view)</t>
-  </si>
-  <si>
-    <t>[ 0.89,  1.07]</t>
-  </si>
-  <si>
-    <t>0.687</t>
-  </si>
-  <si>
-    <t>[  0.92,   1.09]</t>
-  </si>
-  <si>
-    <t>0.530</t>
-  </si>
-  <si>
-    <t>-0.10</t>
-  </si>
-  <si>
-    <t>[-0.25, 0.06]</t>
-  </si>
-  <si>
-    <t>0.885</t>
-  </si>
-  <si>
-    <t>[   0.57,     1.44]</t>
-  </si>
-  <si>
-    <t>0.642</t>
-  </si>
-  <si>
-    <t>[0.48,   1.39]</t>
-  </si>
-  <si>
-    <t>0.759</t>
-  </si>
-  <si>
-    <t>Difference study group 2</t>
-  </si>
-  <si>
-    <t>Difference study group 3</t>
-  </si>
-  <si>
-    <t>Hurdle Within-Person Effects</t>
-  </si>
-  <si>
-    <t>Hu Daily persuasion experienced</t>
-  </si>
-  <si>
-    <t>1.59***</t>
-  </si>
-  <si>
-    <t>[ 1.40,  1.85]</t>
-  </si>
-  <si>
-    <t>Hu Daily persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>1.34***</t>
-  </si>
-  <si>
-    <t>[ 1.19,  1.54]</t>
-  </si>
-  <si>
-    <t>Hu Daily pressure experienced</t>
-  </si>
-  <si>
-    <t>[ 0.69,  1.34]</t>
-  </si>
-  <si>
-    <t>0.587</t>
-  </si>
-  <si>
-    <t>Hu Daily pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>1.48*</t>
-  </si>
-  <si>
-    <t>[ 1.05,  2.28]</t>
-  </si>
-  <si>
-    <t>0.987</t>
-  </si>
-  <si>
-    <t>Hu Daily pushing experienced</t>
-  </si>
-  <si>
-    <t>[ 0.72,  1.31]</t>
-  </si>
-  <si>
-    <t>0.618</t>
-  </si>
-  <si>
-    <t>Hu Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>1.32*</t>
-  </si>
-  <si>
-    <t>[ 1.07,  1.70]</t>
-  </si>
-  <si>
-    <t>Hu Day</t>
-  </si>
-  <si>
-    <t>0.86</t>
-  </si>
-  <si>
-    <t>[ 0.64,  1.16]</t>
-  </si>
-  <si>
-    <t>0.845</t>
-  </si>
-  <si>
-    <t>Hu Daily weartime</t>
-  </si>
-  <si>
-    <t>Hu Actionplan</t>
-  </si>
-  <si>
-    <t>9.97***</t>
-  </si>
-  <si>
-    <t>[ 8.27, 12.04]</t>
-  </si>
-  <si>
-    <t>Hu Daily support received</t>
-  </si>
-  <si>
-    <t>Hu Daily support provided (partner's view)</t>
-  </si>
-  <si>
-    <t>Hu Is a Weekend</t>
-  </si>
-  <si>
-    <t>Hu JITAI received</t>
-  </si>
-  <si>
-    <t>Hu Days post skilled support intervention</t>
-  </si>
-  <si>
-    <t>Hurdle Between-Person Effects</t>
-  </si>
-  <si>
-    <t>Hu Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t>[ 0.61,  2.42]</t>
-  </si>
-  <si>
-    <t>0.721</t>
-  </si>
-  <si>
-    <t>Hu Mean persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>1.09</t>
-  </si>
-  <si>
-    <t>[ 0.55,  2.22]</t>
-  </si>
-  <si>
-    <t>Hu Mean pressure experienced</t>
-  </si>
-  <si>
-    <t>0.43*</t>
-  </si>
-  <si>
-    <t>[ 0.20,  0.94]</t>
-  </si>
-  <si>
-    <t>0.981</t>
-  </si>
-  <si>
-    <t>Hu Mean pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>[ 0.25,  1.19]</t>
-  </si>
-  <si>
-    <t>0.935</t>
-  </si>
-  <si>
-    <t>Hu Mean pushing experienced</t>
-  </si>
-  <si>
-    <t>0.76</t>
-  </si>
-  <si>
-    <t>[ 0.26,  2.25]</t>
-  </si>
-  <si>
-    <t>0.692</t>
-  </si>
-  <si>
-    <t>Hu Mean pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t>1.46</t>
-  </si>
-  <si>
-    <t>[ 0.49,  4.30]</t>
-  </si>
-  <si>
-    <t>Hu Mean weartime</t>
-  </si>
-  <si>
-    <t>Hu Mean support received</t>
-  </si>
-  <si>
-    <t>[ 0.97,  1.53]</t>
-  </si>
-  <si>
-    <t>0.953</t>
-  </si>
-  <si>
-    <t>Hu Mean support provided (partner's view)</t>
-  </si>
-  <si>
-    <t>1.29*</t>
-  </si>
-  <si>
-    <t>[ 1.04,  1.64]</t>
-  </si>
-  <si>
-    <t>0.988</t>
-  </si>
-  <si>
-    <t>Hu Difference study group 2</t>
-  </si>
-  <si>
-    <t>Hu Difference study group 3</t>
-  </si>
-  <si>
-    <t>Random Effects</t>
-  </si>
-  <si>
-    <t>sd(Intercept)</t>
-  </si>
-  <si>
-    <t>0.30</t>
-  </si>
-  <si>
-    <t>[0.23, 0.40]</t>
-  </si>
-  <si>
-    <t>[0.23, 0.39]</t>
-  </si>
-  <si>
-    <t>0.60</t>
-  </si>
-  <si>
-    <t>[0.48, 0.79]</t>
-  </si>
-  <si>
-    <t>0.80</t>
-  </si>
-  <si>
-    <t>[0.46, 1.27]</t>
-  </si>
-  <si>
-    <t>1.14</t>
-  </si>
-  <si>
-    <t>[0.72, 1.75]</t>
-  </si>
-  <si>
-    <t>sd(Hurdle Intercept)</t>
-  </si>
-  <si>
-    <t>0.69</t>
-  </si>
-  <si>
-    <t>[0.52, 0.91]</t>
-  </si>
-  <si>
-    <t>sd(Daily persuasion experienced)</t>
-  </si>
-  <si>
-    <t>0.12</t>
-  </si>
-  <si>
-    <t>[0.08, 0.17]</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>[0.02, 0.08]</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>[0.00, 0.10]</t>
-  </si>
-  <si>
-    <t>0.16</t>
-  </si>
-  <si>
-    <t>[0.01, 0.42]</t>
-  </si>
-  <si>
-    <t>0.20</t>
-  </si>
-  <si>
-    <t>[0.01, 0.51]</t>
-  </si>
-  <si>
-    <t>sd(Daily persuasion utilized (partner's view))</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>[0.04, 0.13]</t>
-  </si>
-  <si>
-    <t>[0.03, 0.09]</t>
-  </si>
-  <si>
-    <t>[0.01, 0.13]</t>
-  </si>
-  <si>
-    <t>[0.01, 0.53]</t>
-  </si>
-  <si>
-    <t>0.48</t>
-  </si>
-  <si>
-    <t>[0.14, 0.96]</t>
-  </si>
-  <si>
-    <t>sd(Daily pressure experienced)</t>
-  </si>
-  <si>
-    <t>[0.00, 0.23]</t>
-  </si>
-  <si>
-    <t>[0.00, 0.13]</t>
-  </si>
-  <si>
-    <t>[0.00, 0.25]</t>
-  </si>
-  <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>[0.09, 1.15]</t>
-  </si>
-  <si>
-    <t>[0.11, 2.42]</t>
-  </si>
-  <si>
-    <t>sd(Daily pressure utilized (partner's view))</t>
-  </si>
-  <si>
-    <t>0.06</t>
-  </si>
-  <si>
-    <t>[0.00, 0.18]</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>[0.00, 0.11]</t>
-  </si>
-  <si>
-    <t>[0.00, 0.27]</t>
-  </si>
-  <si>
-    <t>0.44</t>
-  </si>
-  <si>
-    <t>[0.02, 1.64]</t>
-  </si>
-  <si>
-    <t>[0.05, 2.74]</t>
-  </si>
-  <si>
-    <t>sd(Daily pushing experienced)</t>
-  </si>
-  <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>[0.03, 0.18]</t>
-  </si>
-  <si>
-    <t>[0.01, 0.15]</t>
-  </si>
-  <si>
-    <t>[0.00, 0.14]</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>[0.02, 0.53]</t>
-  </si>
-  <si>
-    <t>0.28</t>
-  </si>
-  <si>
-    <t>[0.03, 0.65]</t>
-  </si>
-  <si>
-    <t>sd(Daily pushing utilized (partner's view))</t>
-  </si>
-  <si>
-    <t>[0.00, 0.09]</t>
-  </si>
-  <si>
-    <t>[0.00, 0.16]</t>
-  </si>
-  <si>
-    <t>[0.01, 0.62]</t>
-  </si>
-  <si>
-    <t>0.26</t>
-  </si>
-  <si>
-    <t>[0.01, 0.95]</t>
-  </si>
-  <si>
-    <t>sd(Hu Daily persuasion experienced)</t>
-  </si>
-  <si>
-    <t>[0.03, 0.41]</t>
-  </si>
-  <si>
-    <t>sd(Hu Daily persuasion utilized (partner's view))</t>
-  </si>
-  <si>
-    <t>0.17</t>
-  </si>
-  <si>
-    <t>[0.01, 0.36]</t>
-  </si>
-  <si>
-    <t>sd(Hu Daily pressure experienced)</t>
-  </si>
-  <si>
-    <t>0.19</t>
-  </si>
-  <si>
-    <t>[0.01, 0.75]</t>
-  </si>
-  <si>
-    <t>sd(Hu Daily pressure utilized (partner's view))</t>
-  </si>
-  <si>
-    <t>0.23</t>
-  </si>
-  <si>
-    <t>[0.01, 0.93]</t>
-  </si>
-  <si>
-    <t>sd(Hu Daily pushing experienced)</t>
-  </si>
-  <si>
-    <t>0.58</t>
-  </si>
-  <si>
-    <t>[0.31, 0.99]</t>
-  </si>
-  <si>
-    <t>sd(Hu Daily pushing utilized (partner's view))</t>
-  </si>
-  <si>
-    <t>[0.01, 0.52]</t>
-  </si>
-  <si>
-    <t>Additional Parameters</t>
-  </si>
-  <si>
-    <t>sigma</t>
-  </si>
-  <si>
-    <t>0.68</t>
-  </si>
-  <si>
-    <t>[0.65, 0.70]</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>[0.56, 0.59]</t>
-  </si>
-  <si>
-    <t>[0.93, 0.98]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="419">
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Subjective MVPA Hurdle Lognormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device-Based MVPA Log (Gaussian)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mood Gaussian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactance Ordinal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactance Dichotome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exp(Est.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95% CI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Est.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38.50***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[33.71, 44.19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">112.69***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[101.42, 125.34]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.66***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 3.44, 3.88]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.32***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.16,   0.61]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurdle Intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.27***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.20,  0.37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Within-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.98,  1.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  1.00,   1.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.04, 0.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.85*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.72,     1.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.70,   1.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.99,  1.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.921</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.99,   1.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.869</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.02, 0.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.83,     1.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.82,   1.52]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.82,  1.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.89,   1.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.14, 0.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.83*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   1.14,     2.59]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.96*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.00,   4.44]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.86,  1.02]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.92,   1.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.15, 0.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.70,     2.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.60,   4.93]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.92,  1.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.97,   1.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.06, 0.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.97,     1.52]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.33*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.02,   1.76]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.91,  1.03]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.96,   1.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.00, 0.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.72,     1.20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.61,   1.35]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.88,  1.12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.91,   1.04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.15, 0.37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.75,     2.89]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.74,   3.49]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.00***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  1.00,   1.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actionplan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.37***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.25,  1.49]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.09**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  1.04,   1.14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.02, 0.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.51,     1.37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.49,   1.43]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily support received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily support provided (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is a Weekend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JITAI received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Days post skilled support intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Between-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.70,  1.29]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.79,   1.41]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.35, 0.80]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.44,     3.81]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.63,   7.27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.75,  1.36]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.73,   1.31]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.27, 0.87]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.46,     5.12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.737</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.53,   7.95]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.87,  1.72]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.77,   1.37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.544</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.81, 0.32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.49*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   1.13,    10.80]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.45**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2.52, 170.41]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.65,  1.33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.73,   1.28]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.89, 0.20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.891</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.35,     3.45]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.583</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.23,  22.98]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.72,  1.90]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.769</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.59,   1.48]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.57, 1.03]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.36,     9.61]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.16,   9.49]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.591</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.65,  1.74]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.73,   1.83]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.62, 1.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.02,     1.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01,   0.84]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean support received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.04,  1.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.98,   1.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.01, 0.30]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.41,     1.31]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.39,   1.46]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean support provided (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.89,  1.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.687</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.92,   1.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.25, 0.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[   0.57,     1.44]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.48,   1.39]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference study group 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference study group 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurdle Within-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.59***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.40,  1.85]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.34***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.19,  1.54]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.69,  1.34]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.48*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.05,  2.28]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.72,  1.31]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.32*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.07,  1.70]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.64,  1.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Actionplan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.97***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 8.27, 12.04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily support received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily support provided (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Is a Weekend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu JITAI received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Days post skilled support intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurdle Between-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.61,  2.42]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.55,  2.22]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.43*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.20,  0.94]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.25,  1.19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.26,  2.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.49,  4.30]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean support received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.97,  1.53]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean support provided (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.29*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 1.04,  1.64]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Difference study group 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Difference study group 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.23, 0.40]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.23, 0.39]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.48, 0.79]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.46, 1.27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.72, 1.75]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hurdle Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.52, 0.91]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily persuasion experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.08, 0.17]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.10]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.42]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.51]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily persuasion utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.04, 0.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.03, 0.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.53]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.14, 0.96]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pressure experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.23]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.09, 1.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.11, 2.42]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pressure utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 1.64]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.05, 2.74]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pushing experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.03, 0.18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.53]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.03, 0.65]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pushing utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.62]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.95]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily persuasion experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.03, 0.41]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily persuasion utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.36]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pressure experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.75]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pressure utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.93]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pushing experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.31, 0.99]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pushing utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.52]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.65, 0.70]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.56, 0.59]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.93, 0.98]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1297,16 +1290,16 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <b/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <i/>
     </font>
   </fonts>
   <fills count="2">
@@ -1326,28 +1319,20 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1363,35 +1348,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1673,83 +1643,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="43.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.40625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.31640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.40625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.40625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.40625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.40625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1799,7 +1750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1843,7 +1794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="4">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1869,58 +1820,58 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A5" s="10" t="s">
+    <row r="5">
+      <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A6" s="7" t="s">
+    <row r="6">
+      <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1969,8 +1920,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A7" s="7" t="s">
+    <row r="7">
+      <c r="A7" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2019,8 +1970,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A8" s="7" t="s">
+    <row r="8">
+      <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2069,8 +2020,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A9" s="7" t="s">
+    <row r="9">
+      <c r="A9" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2119,8 +2070,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A10" s="7" t="s">
+    <row r="10">
+      <c r="A10" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2169,8 +2120,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A11" s="7" t="s">
+    <row r="11">
+      <c r="A11" s="8" t="s">
         <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2219,8 +2170,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A12" s="7" t="s">
+    <row r="12">
+      <c r="A12" s="8" t="s">
         <v>113</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2269,8 +2220,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A13" s="7" t="s">
+    <row r="13">
+      <c r="A13" s="8" t="s">
         <v>126</v>
       </c>
       <c r="B13" s="1"/>
@@ -2295,8 +2246,8 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A14" s="7" t="s">
+    <row r="14">
+      <c r="A14" s="8" t="s">
         <v>129</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -2345,8 +2296,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A15" s="7" t="s">
+    <row r="15">
+      <c r="A15" s="8" t="s">
         <v>143</v>
       </c>
       <c r="B15" s="1"/>
@@ -2365,8 +2316,8 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A16" s="7" t="s">
+    <row r="16">
+      <c r="A16" s="8" t="s">
         <v>144</v>
       </c>
       <c r="B16" s="1"/>
@@ -2385,8 +2336,8 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A17" s="7" t="s">
+    <row r="17">
+      <c r="A17" s="8" t="s">
         <v>145</v>
       </c>
       <c r="B17" s="1"/>
@@ -2405,8 +2356,8 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A18" s="7" t="s">
+    <row r="18">
+      <c r="A18" s="8" t="s">
         <v>146</v>
       </c>
       <c r="B18" s="1"/>
@@ -2425,8 +2376,8 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A19" s="7" t="s">
+    <row r="19">
+      <c r="A19" s="8" t="s">
         <v>147</v>
       </c>
       <c r="B19" s="1"/>
@@ -2445,58 +2396,58 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A20" s="10" t="s">
+    <row r="20">
+      <c r="A20" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="P20" s="11" t="s">
+      <c r="P20" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A21" s="7" t="s">
+    <row r="21">
+      <c r="A21" s="8" t="s">
         <v>149</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2545,8 +2496,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A22" s="7" t="s">
+    <row r="22">
+      <c r="A22" s="8" t="s">
         <v>164</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2595,8 +2546,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A23" s="7" t="s">
+    <row r="23">
+      <c r="A23" s="8" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2645,8 +2596,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A24" s="7" t="s">
+    <row r="24">
+      <c r="A24" s="8" t="s">
         <v>193</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2695,8 +2646,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A25" s="7" t="s">
+    <row r="25">
+      <c r="A25" s="8" t="s">
         <v>208</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2745,8 +2696,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A26" s="7" t="s">
+    <row r="26">
+      <c r="A26" s="8" t="s">
         <v>222</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2795,8 +2746,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A27" s="7" t="s">
+    <row r="27">
+      <c r="A27" s="8" t="s">
         <v>237</v>
       </c>
       <c r="B27" s="1"/>
@@ -2821,8 +2772,8 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A28" s="7" t="s">
+    <row r="28">
+      <c r="A28" s="8" t="s">
         <v>239</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -2871,8 +2822,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A29" s="7" t="s">
+    <row r="29">
+      <c r="A29" s="8" t="s">
         <v>253</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2921,8 +2872,8 @@
         <v>264</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A30" s="7" t="s">
+    <row r="30">
+      <c r="A30" s="8" t="s">
         <v>265</v>
       </c>
       <c r="B30" s="1"/>
@@ -2941,8 +2892,8 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A31" s="7" t="s">
+    <row r="31">
+      <c r="A31" s="8" t="s">
         <v>266</v>
       </c>
       <c r="B31" s="1"/>
@@ -2961,58 +2912,58 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A32" s="10" t="s">
+    <row r="32">
+      <c r="A32" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="J32" s="11" t="s">
+      <c r="J32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="L32" s="11" t="s">
+      <c r="L32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="M32" s="11" t="s">
+      <c r="M32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="N32" s="11" t="s">
+      <c r="N32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="O32" s="11" t="s">
+      <c r="O32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="P32" s="11" t="s">
+      <c r="P32" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A33" s="7" t="s">
+    <row r="33">
+      <c r="A33" s="8" t="s">
         <v>268</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -3037,8 +2988,8 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A34" s="7" t="s">
+    <row r="34">
+      <c r="A34" s="8" t="s">
         <v>271</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -3063,8 +3014,8 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A35" s="7" t="s">
+    <row r="35">
+      <c r="A35" s="8" t="s">
         <v>274</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -3089,8 +3040,8 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A36" s="7" t="s">
+    <row r="36">
+      <c r="A36" s="8" t="s">
         <v>277</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -3115,8 +3066,8 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A37" s="7" t="s">
+    <row r="37">
+      <c r="A37" s="8" t="s">
         <v>281</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -3141,8 +3092,8 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A38" s="7" t="s">
+    <row r="38">
+      <c r="A38" s="8" t="s">
         <v>284</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -3167,8 +3118,8 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A39" s="7" t="s">
+    <row r="39">
+      <c r="A39" s="8" t="s">
         <v>287</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -3193,8 +3144,8 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A40" s="7" t="s">
+    <row r="40">
+      <c r="A40" s="8" t="s">
         <v>291</v>
       </c>
       <c r="B40" s="1"/>
@@ -3213,8 +3164,8 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A41" s="7" t="s">
+    <row r="41">
+      <c r="A41" s="8" t="s">
         <v>292</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -3239,8 +3190,8 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A42" s="7" t="s">
+    <row r="42">
+      <c r="A42" s="8" t="s">
         <v>295</v>
       </c>
       <c r="B42" s="1"/>
@@ -3259,8 +3210,8 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A43" s="7" t="s">
+    <row r="43">
+      <c r="A43" s="8" t="s">
         <v>296</v>
       </c>
       <c r="B43" s="1"/>
@@ -3279,8 +3230,8 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A44" s="7" t="s">
+    <row r="44">
+      <c r="A44" s="8" t="s">
         <v>297</v>
       </c>
       <c r="B44" s="1"/>
@@ -3299,8 +3250,8 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A45" s="7" t="s">
+    <row r="45">
+      <c r="A45" s="8" t="s">
         <v>298</v>
       </c>
       <c r="B45" s="1"/>
@@ -3319,8 +3270,8 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A46" s="7" t="s">
+    <row r="46">
+      <c r="A46" s="8" t="s">
         <v>299</v>
       </c>
       <c r="B46" s="1"/>
@@ -3339,58 +3290,58 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A47" s="10" t="s">
+    <row r="47">
+      <c r="A47" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="G47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I47" s="11" t="s">
+      <c r="I47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="J47" s="11" t="s">
+      <c r="J47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="K47" s="11" t="s">
+      <c r="K47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="L47" s="11" t="s">
+      <c r="L47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="M47" s="11" t="s">
+      <c r="M47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="N47" s="11" t="s">
+      <c r="N47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="O47" s="11" t="s">
+      <c r="O47" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="P47" s="11" t="s">
+      <c r="P47" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A48" s="7" t="s">
+    <row r="48">
+      <c r="A48" s="8" t="s">
         <v>301</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -3415,8 +3366,8 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A49" s="7" t="s">
+    <row r="49">
+      <c r="A49" s="8" t="s">
         <v>304</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -3441,8 +3392,8 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A50" s="7" t="s">
+    <row r="50">
+      <c r="A50" s="8" t="s">
         <v>307</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -3467,8 +3418,8 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A51" s="7" t="s">
+    <row r="51">
+      <c r="A51" s="8" t="s">
         <v>311</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -3493,8 +3444,8 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A52" s="7" t="s">
+    <row r="52">
+      <c r="A52" s="8" t="s">
         <v>315</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -3519,8 +3470,8 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A53" s="7" t="s">
+    <row r="53">
+      <c r="A53" s="8" t="s">
         <v>319</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -3545,8 +3496,8 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A54" s="7" t="s">
+    <row r="54">
+      <c r="A54" s="8" t="s">
         <v>322</v>
       </c>
       <c r="B54" s="1"/>
@@ -3565,8 +3516,8 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A55" s="7" t="s">
+    <row r="55">
+      <c r="A55" s="8" t="s">
         <v>323</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -3591,8 +3542,8 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A56" s="7" t="s">
+    <row r="56">
+      <c r="A56" s="8" t="s">
         <v>326</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -3617,8 +3568,8 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A57" s="7" t="s">
+    <row r="57">
+      <c r="A57" s="8" t="s">
         <v>330</v>
       </c>
       <c r="B57" s="1"/>
@@ -3637,8 +3588,8 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A58" s="7" t="s">
+    <row r="58">
+      <c r="A58" s="8" t="s">
         <v>331</v>
       </c>
       <c r="B58" s="1"/>
@@ -3657,58 +3608,58 @@
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A59" s="10" t="s">
+    <row r="59">
+      <c r="A59" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="H59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="I59" s="11" t="s">
+      <c r="I59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="J59" s="11" t="s">
+      <c r="J59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="K59" s="11" t="s">
+      <c r="K59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="L59" s="11" t="s">
+      <c r="L59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="M59" s="11" t="s">
+      <c r="M59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="N59" s="11" t="s">
+      <c r="N59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="O59" s="11" t="s">
+      <c r="O59" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="P59" s="11" t="s">
+      <c r="P59" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A60" s="7" t="s">
+    <row r="60">
+      <c r="A60" s="8" t="s">
         <v>333</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -3747,8 +3698,8 @@
       </c>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A61" s="7" t="s">
+    <row r="61">
+      <c r="A61" s="8" t="s">
         <v>343</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -3771,8 +3722,8 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A62" s="7" t="s">
+    <row r="62">
+      <c r="A62" s="8" t="s">
         <v>346</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -3811,8 +3762,8 @@
       </c>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A63" s="7" t="s">
+    <row r="63">
+      <c r="A63" s="8" t="s">
         <v>357</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -3851,8 +3802,8 @@
       </c>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A64" s="7" t="s">
+    <row r="64">
+      <c r="A64" s="8" t="s">
         <v>365</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -3891,8 +3842,8 @@
       </c>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A65" s="7" t="s">
+    <row r="65">
+      <c r="A65" s="8" t="s">
         <v>372</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -3931,8 +3882,8 @@
       </c>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A66" s="7" t="s">
+    <row r="66">
+      <c r="A66" s="8" t="s">
         <v>381</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -3971,8 +3922,8 @@
       </c>
       <c r="P66" s="1"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A67" s="7" t="s">
+    <row r="67">
+      <c r="A67" s="8" t="s">
         <v>390</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -4011,8 +3962,8 @@
       </c>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A68" s="7" t="s">
+    <row r="68">
+      <c r="A68" s="8" t="s">
         <v>396</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -4035,8 +3986,8 @@
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A69" s="7" t="s">
+    <row r="69">
+      <c r="A69" s="8" t="s">
         <v>398</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -4059,8 +4010,8 @@
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A70" s="7" t="s">
+    <row r="70">
+      <c r="A70" s="8" t="s">
         <v>401</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -4083,8 +4034,8 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A71" s="7" t="s">
+    <row r="71">
+      <c r="A71" s="8" t="s">
         <v>404</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -4107,8 +4058,8 @@
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A72" s="7" t="s">
+    <row r="72">
+      <c r="A72" s="8" t="s">
         <v>407</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -4131,8 +4082,8 @@
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A73" s="7" t="s">
+    <row r="73">
+      <c r="A73" s="8" t="s">
         <v>410</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4155,58 +4106,58 @@
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A74" s="10" t="s">
+    <row r="74">
+      <c r="A74" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="D74" s="11" t="s">
+      <c r="D74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="E74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="F74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="G74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="H74" s="11" t="s">
+      <c r="H74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I74" s="11" t="s">
+      <c r="I74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="J74" s="11" t="s">
+      <c r="J74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="K74" s="11" t="s">
+      <c r="K74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="L74" s="11" t="s">
+      <c r="L74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="M74" s="11" t="s">
+      <c r="M74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="N74" s="11" t="s">
+      <c r="N74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="O74" s="11" t="s">
+      <c r="O74" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="P74" s="11" t="s">
+      <c r="P74" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A75" s="8" t="s">
+    <row r="75">
+      <c r="A75" s="9" t="s">
         <v>413</v>
       </c>
       <c r="B75" s="4" t="s">
@@ -4237,60 +4188,60 @@
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A76" s="7"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A77" s="7"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A78" s="7"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A79" s="7"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.75">
-      <c r="A80" s="7"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A81" s="7"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A82" s="7"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A83" s="7"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A84" s="7"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A85" s="7"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A86" s="7"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A87" s="7"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A88" s="7"/>
+    <row r="76">
+      <c r="A76" s="8"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="8"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="8"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="8"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="8"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="8"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="8"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="8"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="8"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="8"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="8"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="8"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A74:P74"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="A5:P5"/>
     <mergeCell ref="A20:P20"/>
     <mergeCell ref="A32:P32"/>
     <mergeCell ref="A47:P47"/>
     <mergeCell ref="A59:P59"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="A74:P74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>